<commit_message>
Successfully complete the functions of downloading, filtering, and failure management for book cover images, and form a stable version.
</commit_message>
<xml_diff>
--- a/output/dangdang_books.xlsx
+++ b/output/dangdang_books.xlsx
@@ -492,17 +492,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AI时代生存手册：零基础掌握DeepSeek。deepseek从入门到精通 全网4000万粉丝的AI教育开拓者秋叶匠心之作，解决DeepSeek应用中的各种痛点，瞄准利用DeepSeek发展的各种红利，全方位解锁DS的无限可能</t>
+          <t>企业AI之旅：深度解析AI如何赋能千行百业 DeepSeek时代，深度解析AI如何赋能千行百业，打造企业AI进化路线图。</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>¥29.90</t>
+          <t>¥35.60</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>秋叶 任泽岩 黄震炜</t>
+          <t>[德]拉尔夫·T.克罗伊策（Ralf,T.,Kreutzer）,[德]玛丽·西伦贝格（Marie</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -519,17 +519,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AI时代：弯道超车新思维 李尚龙新书 生物学博士·尹烨、帆书app创始人·樊登；360集团创始人·周鸿祎；硅谷学霸·Jolin联袂推荐！</t>
+          <t>AI短视频生成与制作从入门到精通 人工智能AI短视频教程，ChatGPT＋Midjourney＋文心一格＋腾讯智影＋一帧秒创＋Premiere＋剪映电脑版，文生视频+图生视频+视频生成视频＋AI视频制作＋AI视频应用</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>¥39.80</t>
+          <t>¥49.50</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>李尚龙</t>
+          <t>楚天</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -546,17 +546,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>企业AI之旅：深度解析AI如何赋能千行百业 DeepSeek时代，深度解析AI如何赋能千行百业，打造企业AI进化路线图。</t>
+          <t>AI时代生存手册：零基础掌握DeepSeek。deepseek从入门到精通 全网4000万粉丝的AI教育开拓者秋叶匠心之作，解决DeepSeek应用中的各种痛点，瞄准利用DeepSeek发展的各种红利，全方位解锁DS的无限可能</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>¥35.60</t>
+          <t>¥29.90</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[德]拉尔夫·T.克罗伊策（Ralf,T.,Kreutzer）,[德]玛丽·西伦贝格（Marie</t>
+          <t>秋叶 任泽岩 黄震炜</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -573,17 +573,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AI短视频生成与制作从入门到精通 人工智能AI短视频教程，ChatGPT＋Midjourney＋文心一格＋腾讯智影＋一帧秒创＋Premiere＋剪映电脑版，文生视频+图生视频+视频生成视频＋AI视频制作＋AI视频应用</t>
+          <t>AI时代：弯道超车新思维 李尚龙新书 生物学博士·尹烨、帆书app创始人·樊登；360集团创始人·周鸿祎；硅谷学霸·Jolin联袂推荐！</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>¥49.50</t>
+          <t>¥39.80</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>楚天</t>
+          <t>李尚龙</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -654,15 +654,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>deepseek从入门到精通 AI时代生存手册 真红利</t>
+          <t>与AI同行：我的大模型思考 人工智能绝对是打造新质生产力非常重要的抓手，也是非常重要的历史性机遇。 “红衣大叔”周鸿祎新作</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>¥23.50起</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
+          <t>¥39.50</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>周鸿祎</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>page1_book8.jpg</t>
@@ -677,17 +681,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DeepSeek从入门到精通：打造你的专属AI助手 用DeepSeek打造你的专属AI助手,微软认证专家撰写,体系完备深入浅出,综合30+实战场景,提出5个有效提问法则,6种高效提示词模板,4种DeepSeek+其他工具组合,掌握核心技巧玩转AIGC</t>
+          <t>AI办公新动能:DeepSeek智能应用实践指南 案例视频版 100万+IT畅销书作者专业品质，解锁AI效能不只是提示词 职场焦虑清零，办公效率翻倍！深度定制办公场景，完整构建AI办公思维，覆盖DeepSeek文本、数据、图像、视频全域创作！立体化学习，书+配套视频+拓展课程+丰富资源，附赠8大超值电子资源</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>¥27.60</t>
+          <t>¥39.50</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>彬彬老师 高艺轩</t>
+          <t>关东升</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -704,15 +708,19 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DeepSeek实用操作指南 AI的100个关键 AI时代：弯道超车新思维</t>
+          <t>DeepSeek从入门到精通：打造你的专属AI助手 用DeepSeek打造你的专属AI助手,微软认证专家撰写,体系完备深入浅出,综合30+实战场景,提出5个有效提问法则,6种高效提示词模板,4种DeepSeek+其他工具组合,掌握核心技巧玩转AIGC</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>¥34.90起</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
+          <t>¥27.60</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>彬彬老师 高艺轩</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>page1_book10.jpg</t>
@@ -727,17 +735,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>与AI同行：我的大模型思考 人工智能绝对是打造新质生产力非常重要的抓手，也是非常重要的历史性机遇。 “红衣大叔”周鸿祎新作</t>
+          <t>AI领导力：数字时代领导者的关键能力与核心竞争力 清华大学教授、北大MBA、中科院教授等数十位行业领域专家联袂推荐。书中包含多种原创AI领导力工具，助力企业领导者提升自身能力，完善管理方法。</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>¥39.50</t>
+          <t>¥31.10</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>周鸿祎</t>
+          <t>刘言午</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -754,19 +762,15 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>拐点：站在AI颠覆世界的前夜 身处AI颠覆一切的前夜，如何拿到登上AI大时代的船票？/“文津奖”“中国好书”得主万维钢万Sir，给你一本AI时代的生产手册/以你为主，驾驭AI</t>
+          <t>deepseek从入门到精通 AI时代生存手册 真红利</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>¥49.00</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>万维钢 著; 得到图书 出品</t>
-        </is>
-      </c>
+          <t>¥23.50起</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
           <t>page1_book12.jpg</t>
@@ -781,17 +785,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AI办公新动能:DeepSeek智能应用实践指南 案例视频版 100万+IT畅销书作者专业品质，解锁AI效能不只是提示词 职场焦虑清零，办公效率翻倍！深度定制办公场景，完整构建AI办公思维，覆盖DeepSeek文本、数据、图像、视频全域创作！立体化学习，书+配套视频+拓展课程+丰富资源，附赠8大超值电子资源</t>
+          <t>AI绘画+AI摄影+AI短视频从入门到精通 赠DeepSeek即梦可灵等AI应用指导 生成指令 以文生图 以图生图 AI 75分钟同步教学视频+69个实例案例讲解，免费领取DeepSeek、即梦、可灵等AI应用指导（附赠教学视频），技术与艺术，算法与灵感</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>¥39.50</t>
+          <t>¥39.90</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>关东升</t>
+          <t>新镜界</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -808,17 +812,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DeepSeek实用操作指南 : 入门、搜索、答疑、写作 李尚龙手把手教你用AI DeepSeek，人工智能界的超级英雄、你的专属智能助手，为你开启AI的无限可能！</t>
+          <t>AI超级个体：肖厂长新书，deepseek 时代，掌握AI知识；内容创富的实战方法论 AI时代，内容创富的实战方法论</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>¥48.10</t>
+          <t>¥28.30</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>李尚龙</t>
+          <t>肖逸群 著 大咖书房 出品</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -835,17 +839,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>秒懂AI小红书：7招玩转素人博主变现 秋叶小红书训练营讲师精心打造 结合实际教学经验和学员真实案例 秋叶秒懂AI系列 秒懂AI小红书 内容变现 运营涨粉 获客转化 商业变现 打造IP 引流</t>
+          <t>AI写作宝典： Deepseek 时代，掌握AI写作，10分钟写完3000字 学会AI写作，写文章不求人，零基础教你学会AI写作</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>¥28.70</t>
+          <t>¥29.50</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>有姜姜 李婷儿 王生龙</t>
+          <t>弘丹 著 大咖书房 出品</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -862,17 +866,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>AI短视频制作一本通：文本生成视频+图片生成视频+视频生成视频 超值赠送：DeepSeek 10个高效技巧，即梦、可灵、海螺3款AI短视频制作教程，DS+即梦、DS+剪映AI短视频的制作方法，Sora部署、登陆与视频生成实战</t>
+          <t>真红利:一本书讲透AI时代的风口 2小时掌握AI生存法则 Deepseek 这回真正看懂AI时代的真红利，2小时掌握AI生存法则。</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>¥43.50</t>
+          <t>¥23.50</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>木白 编著</t>
+          <t>秋叶</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -889,17 +893,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>AI领导力：数字时代领导者的关键能力与核心竞争力 清华大学教授、北大MBA、中科院教授等数十位行业领域专家联袂推荐。书中包含多种原创AI领导力工具，助力企业领导者提升自身能力，完善管理方法。</t>
+          <t>AI绘画：Stable Diffusion从入门到精通 AI绘画大潮来袭，创意触手可及！</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>¥31.10</t>
+          <t>¥54.50</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>刘言午</t>
+          <t>许建锋</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -916,17 +920,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>AI时代，学什么，怎么学 清华大学理学博士、人大附中和渊老师解读AI时代学习法，教你掌握未来世界核心竞争力，该如何正确、有效地使用人工智能工具，无需焦虑，这本书让你不掉队。</t>
+          <t>AI赋能企业数字化转型 深入探讨数字化理念精髓，全面解构数字化转型框架。</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>¥39.90</t>
+          <t>¥33.50</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>和渊</t>
+          <t>常耀斌</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -943,19 +947,15 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AI量化之道：DeepSeek+Python让量化交易插上翅膀 AI量化保姆级案例教程：DeepSeek赋能，50个真实实战案例，教你轻松玩转量化交易。</t>
+          <t>DeepSeek实用操作指南 AI的100个关键 AI时代：弯道超车新思维</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>¥61.40</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>关东升 著</t>
-        </is>
-      </c>
+          <t>¥34.90起</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
           <t>page1_book19.jpg</t>
@@ -970,17 +970,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>真红利:一本书讲透AI时代的风口 2小时掌握AI生存法则 Deepseek 这回真正看懂AI时代的真红利，2小时掌握AI生存法则。</t>
+          <t>拐点：站在AI颠覆世界的前夜 身处AI颠覆一切的前夜，如何拿到登上AI大时代的船票？/“文津奖”“中国好书”得主万维钢万Sir，给你一本AI时代的生产手册/以你为主，驾驭AI</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>¥23.50</t>
+          <t>¥49.00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>秋叶</t>
+          <t>万维钢 著; 得到图书 出品</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -997,17 +997,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>AI公文写作 从提笔犯难到高效成文 20多种AI工具组合应用，让你掌握“怎么写”和“为什么这样写”，助力公文写作与职场思维双重提升。</t>
+          <t>你好，AI：智能时代职场生存指南（为现代职场人量身打造的AI实用指南，帮助读者从对AI的初步认知，进阶到灵活运用Deep</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>¥37.80</t>
+          <t>¥23.20</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>许晓波</t>
+          <t>憨爸，胡斌</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1024,17 +1024,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>漫画AI趣味物理 与ai同行启蒙 孩子爱看的漫画趣味百科 小四门课外阅读书</t>
+          <t>AI轻创业:从零开始学做一人公司 用AI开始你的一人公司 打造可持续</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>¥22.80</t>
+          <t>¥33.10</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>中国纺织出版社</t>
+          <t>谭泽兴</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1051,17 +1051,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>漫画AI趣味化学 与ai同行启蒙 孩子爱看的漫画趣味百科 小四门课外阅读书</t>
+          <t>AI运营新引擎：DeepSeek驱动7大平台爆款打造与变现实战（案例视频版）自媒体变现实操手册 新媒体运营爆款指南 De</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>¥22.80</t>
+          <t>¥44.50</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>中国纺织出版社</t>
+          <t>刘忠彬 编著</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1078,17 +1078,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>AI实操：引流变现8步法 北大、清华特聘AI导师、阿里铁军新媒体带货应用发起人、亿级直播操盘手 武建伟（武大侠）400亿+业绩AI实战经验总结 AI数字员工营销陪跑专家手把手教你AI引流、获客、变现 AI+文案/短视频/投放</t>
+          <t>穿越AI时代的36个思维工具 万维钢、吴晓波、罗振宇、席酉民 鼎力推荐，一本直指AI时代人类底层优势的工具书 万维钢、吴晓波、罗振宇、席酉民 鼎力推荐 一本直指AI时代「人类」底层优势的工具书</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>¥59.80</t>
+          <t>¥34.00</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>武建伟</t>
+          <t>钱自严 著,博集天卷 出品</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1105,17 +1105,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>AI超级个体：肖厂长新书，deepseek 时代，掌握AI知识；内容创富的实战方法论 AI时代，内容创富的实战方法论</t>
+          <t>AI时代的混合动力：AI领导力+企业AI之旅（套装2册）领导者的AI必修课，从管理思维升级到业务落地路径，一站式解决 A 当 AI 领导力教会你用技术思维管人，企业 AI 之旅正揭开零售 / 医疗等 8 大行业转型密码：两本书把‘管理者认知升级’和‘企业技术落地’讲透，让 AI 从概念变成赚钱工具！</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>¥28.30</t>
+          <t>¥66.60</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>肖逸群 著 大咖书房 出品</t>
+          <t>刘言午，[德]拉尔夫·T.克罗伊策(Ralf T. Kreutzer)，[德]玛丽·西伦贝格({</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1132,17 +1132,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>AI绘画+AI摄影+AI短视频从入门到精通 赠DeepSeek即梦可灵等AI应用指导 生成指令 以文生图 以图生图 AI 75分钟同步教学视频+69个实例案例讲解，免费领取DeepSeek、即梦、可灵等AI应用指导（附赠教学视频），技术与艺术，算法与灵感</t>
+          <t>AI音乐家：三天打造自己的音乐专辑</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>¥39.90</t>
+          <t>¥27.60</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>新镜界</t>
+          <t>刘武斌</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1159,17 +1159,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>AI写作宝典： Deepseek 时代，掌握AI写作，10分钟写完3000字 学会AI写作，写文章不求人，零基础教你学会AI写作</t>
+          <t>DeepSeek实用操作指南 : 入门、搜索、答疑、写作 李尚龙手把手教你用AI DeepSeek，人工智能界的超级英雄、你的专属智能助手，为你开启AI的无限可能！</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>¥29.50</t>
+          <t>¥34.90</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>弘丹 著 大咖书房 出品</t>
+          <t>李尚龙</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1186,17 +1186,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>剪映：即梦AI绘画与视频制作从新手到高手 超值赠送：DeepSeek 10个高效技巧，即梦、可灵、海螺3款AI短视频制作教程，DS+即梦、DS+剪映AI短视频的制作方法，Sora部署、登陆与视频生成实战</t>
+          <t>秒懂AI小红书：7招玩转素人博主变现 秋叶小红书训练营讲师精心打造 结合实际教学经验和学员真实案例 秋叶秒懂AI系列 秒懂AI小红书 内容变现 运营涨粉 获客转化 商业变现 打造IP 引流</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>¥44.50</t>
+          <t>¥28.70</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>向秋 编著</t>
+          <t>有姜姜 李婷儿 王生龙</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1213,17 +1213,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>AI绘画：Stable Diffusion从入门到精通 AI绘画大潮来袭，创意触手可及！</t>
+          <t>AI学习助手：给青少年的DeepSeek快速入门指南 专为中小学生量身打造的全学科学习神器 专为中小学生量身打造的全学科“学习神器” 家长省心省力，孩子学的开心，成绩提升轻松。</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>¥54.50</t>
+          <t>¥25.00</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>许建锋</t>
+          <t>图蓝 赛启团队 著 王娜 绘</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1240,15 +1240,19 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>人工智能AI 我看见的世界 李飞飞自传 人工智能时代与人类未来 基辛格科技前沿未来世界AI</t>
+          <t>AI短视频制作一本通：文本生成视频+图片生成视频+视频生成视频 超值赠送：DeepSeek 10个高效技巧，即梦、可灵、海螺3款AI短视频制作教程，DS+即梦、DS+剪映AI短视频的制作方法，Sora部署、登陆与视频生成实战</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>¥45.30</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr"/>
+          <t>¥43.50</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>木白 编著</t>
+        </is>
+      </c>
       <c r="D31" t="inlineStr">
         <is>
           <t>page1_book30.jpg</t>
@@ -1263,17 +1267,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>AI赋能企业数字化转型 深入探讨数字化理念精髓，全面解构数字化转型框架。</t>
+          <t>用AI做副业赚钱 快!别人都在用AI偷偷变富了! 你还在等什么? 在流量见顶的时代，还有哪些机会留给普通人？ 大白话+手把手教学，让普通人也能用AI做副业赚钱!</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>¥33.50</t>
+          <t>¥26.90</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>常耀斌</t>
+          <t>李牧远 著</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1290,17 +1294,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>AI新媒体运营：文案写作＋图片创作＋视频制作＋营销推广从入门到精通 全链路运营指南，深度解析DeepSeek、Kimi、豆包等10多个爆款AI工具，涵盖文案、图片、视频、音乐、数据、投流、变现等场景</t>
+          <t>剪映AI：短、中、长视频剪辑全攻略（手机版+电脑版+网页版） AI赋能剪映，3秒智能成片，7步专业级制作；一个软件，三个版本，三种视频，全面精通。</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>¥57.70</t>
+          <t>¥44.90</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>全权 编著</t>
+          <t>沈沛</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1317,17 +1321,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>AI重塑生意经：如何实现快速盈利 一本书教老板们如何利用AI从0到1低风险创业、赚钱，内含AI提问模板及9大经商要点，帮助做生意的人解决经商难题，让AI重塑生意，实现降本增效与经商成功。</t>
+          <t>AI时代生存手册零基础掌握DeepSeek秋叶+李尚龙签章版DeepSeek实用操作指南 共2册 手把手教你用AI de 新华书店正版，关注店铺成为会员可享店铺专属优惠，团购客户请咨询在线客服！</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>¥55.10</t>
+          <t>¥58.10</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>莫敏、宋涛、刘巨波、苏嵩</t>
+          <t>秋叶 任泽岩 黄震炜</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1344,17 +1348,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>AI领航：无限升维=AI：The Only Way is UP</t>
+          <t>AI时代生存手册 零基础掌握DeepSeek 秋叶 任泽岩 黄震炜 deepseek从入门到精通 轻松上手DeepSee 新华书店正版，关注店铺成为会员可享店铺专属优惠，团购客户请咨询在线客服！</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>¥57.40</t>
+          <t>¥24.80</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>世界人工智能大会《WAIC UP！》编辑部</t>
+          <t>秋叶,任泽岩,黄震炜</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1371,17 +1375,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>AI辅助教学创新：课程设计、成果建设与项目申报 "肯学君"主理人新作 37个应用热点讲透教学创新 涵盖课程设计 成果建设与项目申报</t>
+          <t>AI未来进行式 李开复 陈楸帆 著 人工智能元宇宙 预测接近真实的科技未来 解析未来20年人工智能等科技发展趋势 新华书店正版，关注店铺成为会员可享店铺专属优惠，团购客户请咨询在线客服！</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>¥61.40</t>
+          <t>¥38.60</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>姚飞</t>
+          <t>李开复,陈楸帆</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1398,17 +1402,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>AI绘画：Midjourney从入门到精通 靳太然 人工智能绘画学习书籍 零基础入门教程 保姆级教程</t>
+          <t>AI未来进行式 李开复杨澜俞敏洪洪晃荐解析未来20年人工智能等科技发展趋势预测接近真实的科技未来正版当当自营未来进行</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>¥66.70</t>
+          <t>¥44.00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>靳太然</t>
+          <t>李开复 陈楸帆</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1425,17 +1429,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>AI管理学：人工智能重塑企业管理</t>
+          <t>AI未来进行式 浙江人民出版社 新华书店正版，关注店铺成为会员可享店铺专属优惠，团购客户请咨询在线客服！</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>¥85.30</t>
+          <t>¥39.10</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>董本洪</t>
+          <t>李开复,陈楸帆</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1452,17 +1456,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>AI摄影创作实战 Midjourney指令AI照片生成Photoshop与像素蛋糕修图全解 AI生成式摄影指令教学，Midjourney、Photoshop、像素蛋糕AI修图快速上手，附赠视频和素材</t>
+          <t>AI时代人性的弱点（Thinkers50年度新管理图书，让你在AI时代重拾人类独一无二的价值） 揭示人类智能与AI互动中的典型表现，分析当前AI技术发展进入的错误方向；全球50大管理思想家年度新管理图书；澳大利亚前总理、畅销书《四千周》作者力荐；中资海派出品</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>¥70.30</t>
+          <t>¥34.90</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>杨志</t>
+          <t>［英］托马斯·查莫罗-普雷穆季奇（Tomas,Chamorro-Premuzic） 著；李文远</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1479,17 +1483,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>AI传媒学：大模型助力传媒行业应用与创新</t>
+          <t>AI 改变世界：人工智能新发展与智算经济 走向智能未来的最新探索指南</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>¥76.40</t>
+          <t>¥39.60</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>刘志红</t>
+          <t>方磊 黄郑</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1506,17 +1510,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>你好，AI：智能时代职场生存指南（为现代职场人量身打造的AI实用指南，帮助读者从对AI的初步认知，进阶到灵活运用Deep</t>
+          <t>AI的100个关键：deepseek的底层逻辑 李尚龙著 深入浅出解读AI，从原理到应用，从挑战到机遇，带你全方位领略人工智能的精彩世界！</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>¥23.20</t>
+          <t>¥34.90</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>憨爸，胡斌</t>
+          <t>李尚龙</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1533,17 +1537,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>AI创业狂想曲 20余位AI创业领军人物亲述创业历程，不仅是一部创业实录，更是一份AI时代的战略地图，视觉中国总裁柴继军|真格基金管理合伙人 戴雨森|果壳CEO 姬十三|知乎创始人、CEO 周源等众多专家联袂赞誉</t>
+          <t>AI产品经理手册 打造DeepSeek级AI产品！以AI驱动产品革新，快速学习AI技术认知和产品管理方法！</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>¥48.40</t>
+          <t>¥29.90</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Yuca Hong（洪钰钏）等</t>
+          <t>[美] 艾琳·布拉西斯（Irene Bratsis）着 张玉君 刘璐 译</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1560,17 +1564,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>AI+Photoshop智能图像处理</t>
+          <t>AI爆款文案：AI时代的流量密码，你的心灵成长指南 李尚龙著 AI写爆款,让写作变得更快、更赚、更简单 让AI点燃你的创作灵感，轻松打造10万+爆款 AI写作变现，用AI让你的文字价值百万 教你轻松驾驭智能AI，新手小白也能成为创作大师</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>¥61.60</t>
+          <t>¥34.90</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>葛文艳 主编，岳静茹、杨雪 副主编</t>
+          <t>李尚龙著</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1587,17 +1591,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>AI文明史·前史 亚洲图书奖得主张笑宇新作 刘擎 俞敏洪 罗振宇等推荐 亚洲图书奖得主、新锐科技史学者 张笑宇 重磅作品！何怀宏、刘擎、俞敏洪、罗振宇等推荐。</t>
+          <t>AI Agent开发与应用：基于大模型的智能体构建</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>¥57.90</t>
+          <t>¥49.50</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>张笑宇</t>
+          <t>凌峰</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1614,17 +1618,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>AI共生指南：技术探索与人文思考</t>
+          <t>AI动漫一本通：三分钟速通影视+动漫+设计创作</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>¥54.40</t>
+          <t>¥27.60</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>林亦</t>
+          <t>李源</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1641,17 +1645,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>AI芯片：科技探索与AGI愿景 揭示打造下一代AI 芯片的关键路径 绘制未来的AI 芯片设计全景图</t>
+          <t>AI驱动下的量化策略构建（微课视频版） 配套教学课件，100个示例源代码，213分钟视频讲解 资深量化工程师手把手教你利用AI搭建量化策略 系统讲解AI应用于投研搭建、数据挖掘、量化策略和实盘</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>¥155.20</t>
+          <t>¥54.50</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>张臣雄</t>
+          <t>江建武、季枫、梁举</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1668,17 +1672,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>AI赋能高校辅导员</t>
+          <t>如何向AI提问 精准提问，让DeepSeek的回答更优质 不会提问，再强大的AI工具也帮不了你。万能提问公式+超全场景对比案例，一本技术使用指南兼思维训练手册，教你学会用高效提问解锁AI“超能力”！</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>¥68.80</t>
+          <t>¥23.20</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>杨东杰，闫亮亮</t>
+          <t>晴山 易兴 著 时代华语 出品</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1695,17 +1699,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>穿越AI时代的36个思维工具 万维钢、吴晓波、罗振宇、席酉民 鼎力推荐，一本直指AI时代人类底层优势的工具书 万维钢、吴晓波、罗振宇、席酉民 鼎力推荐 一本直指AI时代「人类」底层优势的工具书</t>
+          <t>AI+人力资源管理：HR进阶实践（新时代·管理新思维） AI+HR最大化激发人才价值，多角度赋能HR加快转型升级。AI与HR工作多个环节融合，有效推动工作流程简化优化；智能系统实现高效自动决策，贴心关怀提升员工工作体验。</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>¥34.00</t>
+          <t>¥33.10</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>钱自严 著,博集天卷 出品</t>
+          <t>梁咏峰</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1722,7 +1726,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>AI轻创业:从零开始学做一人公司 用AI开始你的一人公司 打造可持续</t>
+          <t>AI育儿</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1732,7 +1736,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>谭泽兴</t>
+          <t>刘燕旎</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1749,17 +1753,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>AI赋能Revit建筑创新设计（Revit 2024）（视频教学版） Revit+AI 建筑设计从入门到进阶 新手基础教程 + AI 高级技巧实战指南 附最佳实践案例</t>
+          <t>AI短视频生成与剪辑实战108招：ChatGPT+剪映 赠送Deepseek、即梦、可灵、kimi、通义、文心一言、秘塔等工具的使用指导，70多个案例关键词+108招干活技巧，实操实练，秒变AI视频高手</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>¥62.30</t>
+          <t>¥44.90</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>高珍宇</t>
+          <t>蒋珍珠</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1776,17 +1780,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>AI引爆流量变现IP打造与商业变现实战 AI工具赋能商业、企业、个人IP打造与变现，提供9种实用工具+20个核心场景教学+课程，打通公域引流与私域转化闭环</t>
+          <t>AI赋能小红书运营：爆款打造+推广引流+店铺运营+品牌战略+实操案例 以Deepseek等AI工具结合小红书算法等专业运营，实现从0到1运营小红书</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>¥47.50</t>
+          <t>¥28.70</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>焱公子 水青衣</t>
+          <t>符健治</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1803,17 +1807,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>AI全域营销：打造持续盈利的增长引擎 让AI赋能企业及个人营销，6个环节提升营销业绩，产品诊断、赛道选择、传播矩阵、成交矩阵、私域裂变，多行业实战案例拆解，工具即学即用。</t>
+          <t>AI赋能演讲：关键时刻讲出影响力（新时代·职场新技能） 8种关键演讲场景；50+表达模型；100+应用实例精华。 AI赋能演讲，全面提升你的演讲逻辑力与说服力！</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>¥47.50</t>
+          <t>¥33.10</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>王静，洪海江</t>
+          <t>田楠 著</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1830,17 +1834,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>AI赋能公文写作（新时代·职场新技能） DeepSeek、Kimi、豆包、通义千问、智谱清言、天工和秘塔，解决材料痛点的新路径。既用AI写材料，更用AI学习写材料40+真实案例，展示AI工具与“大秘”文笔的绝妙融合。</t>
+          <t>AI提问之道：不会提问，怎么玩AI ai书籍、ai提问、ai交互、chatgpt、kimi、ai提示词、提示工程、pro</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>¥46.90</t>
+          <t>¥29.90</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>伏虎 王振</t>
+          <t>杜光明</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1857,17 +1861,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>AI辅助设计：图像合成与广告海报创意制作商业应用 40个实战案例，Midjourney、Stable Diffusion从入门到精通</t>
+          <t>AI助力教学：让中小学教师工作更高效</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>¥76.40</t>
+          <t>¥49.50</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>雷波 编著</t>
+          <t>黎渝幸 著</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1884,17 +1888,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>AI应用全能手：文案写作+学习办公+生活咨询+绘图设计+音乐视频+电商运营 AI场景案例应用大全，助您高效提升职场办公与生活</t>
+          <t>AI提示工程必知必会 让AI成为你的高效助理，用好DeepSeek提示词，走上开挂人生，适合各层次读者</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>¥68.60</t>
+          <t>¥44.50</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>张梦琪 编著</t>
+          <t>王国平</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1911,17 +1915,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>AI大模型系统开发技术 一书读懂大模型，了解大模型的很好的读物</t>
+          <t>AI智能写作助手：创作技巧、内容优化与科研应用 AI辅助论文写作，AI提示词高效使用范例大全；ChatGPT学术创作技巧</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>¥43.50</t>
+          <t>¥30.60</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>鞠时光，周从华，宋香梅，王秀红</t>
+          <t>王常圣、李强、汪正斌 著</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1938,17 +1942,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>AI赋能制造业价值链重构</t>
+          <t>AI智能办公实战108招：ChatGPT+Word+PowerPoint+WPS 赠送Deepseek、即梦、可灵、kimi、通义、文心一言、秘塔等工具的使用指导，一本书在手，AI智能办公信手拈来</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>¥64.20</t>
+          <t>¥44.90</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>章丽萍</t>
+          <t>曾公子</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1965,17 +1969,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>AI智能化办公：DeepSeek使用方法与技巧从入门到精通 基础上手，助你快速精通：认识DeepSeek大模型→基本操作→高效撰写文稿→高效处理与分析数据→高效制作PPT→辅助学术研究→赋能AI绘图与视频创作→变身生活多面助手→深度推理逻辑</t>
+          <t>AI写作：爆款文案从入门到精通 一本书精通ChatGPT、文心一言两大AI文案创作工具！快速掌握AI文案写作180招，获取爆款文案创作灵感！超值赠送教学视频、DeepSeek应用技巧及教学课件</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>¥57.70</t>
+          <t>¥28.70</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>李婕,高博 著</t>
+          <t>叶龙</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1992,17 +1996,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>AI提问之道：DeepSeek提示工程入门与实践 北京大学出版社 效率100倍提升宝典：零基础构建AI底层应用逻辑，玩转AI提问技巧，任何领域的小白也能秒变高手</t>
+          <t>AI进行时：AI时代人性的弱点+当我点击时算法在想什么（套装2册） 揭示人类智能与AI互动中的典型表现，分析当前AI技术发展进入的错误方向；硬核数学家、“数学及其应用协会”凯瑟琳·理查兹奖得主力作，破除AI崇拜的诚意之作，重塑大众对人工智能的认知</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>¥57.70</t>
+          <t>¥69.80</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>夏禹,赖晖,李冰玉 著</t>
+          <t>[英]托马斯·查莫罗-普雷穆季奇，[瑞典]大卫·萨普特</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2019,17 +2023,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>AI必修课：从全面理解到高效应用 一本书，轻松理解AI，用好AI，用对AI；全面掌握AI，快速提升生活和工作效率。</t>
+          <t>AI短视频创作与剪辑从入门到实践(微视频版) 随书提供书中案例操作视频、素材文件等配套资源，获取地址见书内容简介网址，或前言和封底二维码。教材服务QQ：1815317009。</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>¥77.20</t>
+          <t>¥44.50</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>[美]迈克尔·米勒（Michael Miller）著 周靖 译</t>
+          <t>李莹、宋岩峰、王嘉熠</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2046,15 +2050,19 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>基于AI的Web技术项目实战（普通高等教育计算机类专业教材）</t>
+          <t>AI+3ds Max 2025从新手到高手（微课版） 全彩印刷 72个视频，时长超过7小时</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>¥44.20</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr"/>
+          <t>¥49.50</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>来阳</t>
+        </is>
+      </c>
       <c r="D61" t="inlineStr">
         <is>
           <t>page1_book60.jpg</t>
@@ -2115,17 +2123,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AI时代自媒体手册：deepseek从入门到精通 用AI成就IP</t>
+          <t>AI短视频创作一本通： 剪映+即梦+即创+可灵+腾讯智影+文心一言+AI数字人 6大AI工具，·49个实战案例，470多张图片，AI短视频制作全掌握！</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>¥43.70</t>
+          <t>¥39.00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>丁玥</t>
+          <t>郝倩 著</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2142,17 +2150,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AI时代的混合动力：AI领导力+企业AI之旅（套装2册）领导者的AI必修课，从管理思维升级到业务落地路径，一站式解决 A 当 AI 领导力教会你用技术思维管人，企业 AI 之旅正揭开零售 / 医疗等 8 大行业转型密码：两本书把‘管理者认知升级’和‘企业技术落地’讲透，让 AI 从概念变成赚钱工具！</t>
+          <t>AI教育行业应用从入门到精通 多种配套资源，30多个AI教育工具，搭配80个实战案例解析。</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>¥66.60</t>
+          <t>¥28.70</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>刘言午，[德]拉尔夫·T.克罗伊策(Ralf T. Kreutzer)，[德]玛丽·西伦贝格({</t>
+          <t>谭先</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2169,17 +2177,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AI+SolidWorks 2024完全实训手册 超值赠送 86个视频教学，时长超过22小时</t>
+          <t>AI数学</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>¥66.20</t>
+          <t>¥23.20</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>李伟 杨秀丽 王岩</t>
+          <t>丛日明, 姜添耀, 丛心尉, 编著</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2196,17 +2204,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AI大模型助你轻松搞定数据分析 AI+数据分析双重技能，通过大量真实工作场景案例，拿来即用的分析报告模板，激发你的数据思维、结构化思考能力。</t>
+          <t>AI办公助手 ChatGPT+Office智能办公从入门到实践（80集视频课） 人工智能时代，AI+ChatGPT助力Word、Excel、PPT智能高效办公，提高工作效率，提升职场竞争力</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>¥93.40</t>
+          <t>¥39.90</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>吴昙</t>
+          <t>宫祺</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2223,17 +2231,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AI大模型企业落地指南 提供企业大模型落地的战略规划、实施步骤和注意事项，助力企业把握科技发展先机。</t>
+          <t>AI化学与生物 口袋里的人工智能 人工智能知识启蒙科普读物 AI技术应用化学生物应用化学合成蛋白质结构基因调控新材料预测 从大众科普的角度，对人工智能在化学、生物领域的应用进行了阐述</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>¥54.50</t>
+          <t>¥16.60</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>贾利阳 王奇</t>
+          <t>陈俊龙 马晶</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2250,17 +2258,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AI音乐家：三天打造自己的音乐专辑</t>
+          <t>AI大模型开发之路：从入门到实践 内容全面，由浅入深，实战案例丰富，一本全面探索人工智能大模型开发领域的实用指南</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>¥27.60</t>
+          <t>¥44.90</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>刘武斌</t>
+          <t>谢雪葵</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2277,17 +2285,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AI量化交易：高效构建交易策略的新路径 AI量化交易里程碑之作：零基础友好，轻松上手并复现专业工作流，15套策略开箱即用！国务院特殊津贴专家杨晓光等产学界专家推荐|附送超值AI量化交易资源</t>
+          <t>AI数字孪生建模与计算 基于AI和物理模型集成，从动态视觉全面、深入介绍建模，填补了数字孪生领域空白，并为模型可解释性提供了新范式。参考文献请扫封底二维码下载。</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>¥77.20</t>
+          <t>¥34.00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>罗勇 卢洪波 王光伟 罗天奇</t>
+          <t>[美] 兰詹·甘古里, 桑迪蓬·阿迪卡里, 苏维克·查克拉博蒂, 姆里蒂卡·甘古利</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2304,17 +2312,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>AI运营新引擎：DeepSeek驱动7大平台爆款打造与变现实战（案例视频版）自媒体变现实操手册 新媒体运营爆款指南 De</t>
+          <t>AI办公助理：让职场效率倍增的16大国产AI工具手册 国产AI大模型工具应用技巧大全，助力工作效率起飞！</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>¥44.50</t>
+          <t>¥44.60</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>刘忠彬 编著</t>
+          <t>柏先云 编著</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2331,17 +2339,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>AI应用进阶系列：图表说营销</t>
+          <t>AI虚拟数字人：商业模式+形象创建+视频直播+案例应用 从AI虚拟数字人的概况、价值与模式，到创作平台、制作软件、行业应用，一应俱全。</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>¥65.00</t>
+          <t>¥44.90</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>张建南</t>
+          <t>李军仁</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2358,17 +2366,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>AI全能应用七合一：ChatGPT+DALL·E+Midjourney+SD+PS+剪映+可灵 轻松驾驭文本、图像、视频创作，实现跨领域应用与商业价值！</t>
+          <t>AI可解释性（Python语言版） DeepSeek知识储备,通过构建XAI的方法论体系，形成一组工具和方法，从而解释ML模型产生的复杂结果，帮助人们理解ML模型。</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>¥76.40</t>
+          <t>¥29.90</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>谢智博 著</t>
+          <t>[意] 列奥尼达·詹法纳(Leonida Gianfagna)、安东尼奥·迪·塞科(Antonio Di Cecco)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2385,17 +2393,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AI时代的认知突围指南系列3册套装：主见+思考如何超越思考+把思考作为习惯</t>
+          <t>AI绘画：Stable Diffusion ComfyUI的艺术</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>¥224.20</t>
+          <t>¥49.50</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>［美］维克拉姆·曼沙拉马尼（Vikram Mansharamani） 著，陆霓 译，湛庐文化 出品</t>
+          <t>许建锋</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2412,17 +2420,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AI短视频制作完全攻略(全面解析AI短视频创作5大核心技法) 保姆级AI短视频制作教程：从文案生成到智能剪辑，一本书掌握AI创作全链条，实现效率100倍提升。</t>
+          <t>AI数据处理实战108招：ChatGPT+Excel+VBA 一本书在手，AI数据处理信手拈来！</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>¥35.80</t>
+          <t>¥44.90</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>时代飞鹰 编著</t>
+          <t>曾公子</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2439,17 +2447,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AI时代生存手册零基础掌握DeepSeek秋叶+李尚龙签章版DeepSeek实用操作指南 共2册 手把手教你用AI de 新华书店正版，关注店铺成为会员可享店铺专属优惠，团购客户请咨询在线客服！</t>
+          <t>AI+Maya 2025从新手到高手（微课版） 全彩印刷 73个视频 时长超过8小时</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>¥58.10</t>
+          <t>¥49.50</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>秋叶 任泽岩 黄震炜</t>
+          <t>来阳</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2466,17 +2474,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>AI时代学什么怎么学 解读AI时代学习法 掌握未来核心竞争力 不被淘汰 和渊著 高盈绘 如何领先一步转变思路 家庭教育育 新华书店正版，关注店铺成为会员可享店铺专属优惠，团购客户请咨询在线客服！</t>
+          <t>AI办公应用实战一本通：AIGC 10大工具应用全案 用AIGC工具提升工作效率，涵盖国内10大主流AIGC工具，岗位典型应用场景,将细节讲清楚。</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>¥35.60</t>
+          <t>¥49.00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>和渊</t>
+          <t>绘蓝书源 著</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -2493,17 +2501,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>AI时代生存手册 零基础掌握DeepSeek 秋叶 任泽岩 黄震炜 deepseek从入门到精通 轻松上手DeepSee 新华书店正版，关注店铺成为会员可享店铺专属优惠，团购客户请咨询在线客服！</t>
+          <t>AI虚拟数字人从入门到精通 5大流行AI工具+200分钟教学视频+3大类商业案例，轻松上手制作AI数字人</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>¥24.80</t>
+          <t>¥34.90</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>秋叶,任泽岩,黄震炜</t>
+          <t>谷建阳</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -2520,17 +2528,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>AI实操：引流变现8步法+手机短视频拍摄与创意剪辑实战（全2册）AI数字员工营销陪跑专家手把手教你AI引流、获客、变现 AI数字员工营销陪跑专家手把手教你 AI引流、获客、变现，拍照手机选择·常用设备·拍摄姿势·拍摄构图 抖音短视频创作·Premiere 创意剪辑·短视频分享</t>
+          <t>AI绘画工坊：Midjourney从入门到实践（80集视频课+50个绘画案例） Midjourney AI绘画商用实战手册！50个AI绘画案例，带你拓展思路，激发创意，开启设计新篇章！</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>¥94.60</t>
+          <t>¥59.00</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>罗巨浪、周冰渝、陈静茹</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2547,17 +2555,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>AI未来进行式 李开复 陈楸帆 著 人工智能元宇宙 预测接近真实的科技未来 解析未来20年人工智能等科技发展趋势 新华书店正版，关注店铺成为会员可享店铺专属优惠，团购客户请咨询在线客服！</t>
+          <t>AI高效制作PPT 从PPT小白到演示大师</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>¥38.60</t>
+          <t>¥17.90</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>李开复,陈楸帆</t>
+          <t>朱晔，郭泽德，蔡洁 著</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2574,17 +2582,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>AI时代人性的弱点（Thinkers50年度新管理图书，让你在AI时代重拾人类独一无二的价值） 揭示人类智能与AI互动中的典型表现，分析当前AI技术发展进入的错误方向；全球50大管理思想家年度新管理图书；澳大利亚前总理、畅销书《四千周》作者力荐；中资海派出品</t>
+          <t>AI作文-小学生获奖作文大全 老师推荐3三4四5五6六年级语文作文训练辅导书 优秀作文选范文大全 小学生满分类获奖作文起</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>¥34.90</t>
+          <t>¥7.50</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>［英］托马斯·查莫罗-普雷穆季奇（Tomas,Chamorro-Premuzic） 著；李文远</t>
+          <t>桂帜明 著</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2601,19 +2609,15 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>少年学AI，看这本就够了 零基础掌握DeepSeek 人工智能入门与实战书籍 青少年编程思维训练 机器学习实战 未来科技</t>
+          <t>围棋AI定式后续策略</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>¥29.80</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>武育泰</t>
-        </is>
-      </c>
+          <t>¥26.10</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
           <t>page2_book19.jpg</t>
@@ -2628,17 +2632,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>AI通识课12讲：走进人工智能 12堂硬核通识课，拆解AI感官、思维与创造力，重构教育、就业与人性认知！</t>
+          <t>AI设计+PS电商美工：文案绘图+抠图修图+场景合成+视频制作 电商文案、商品图图、详情页、模特、虚拟数字人主播、主图视频一站式讲解</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>¥53.40</t>
+          <t>¥44.00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>包坤</t>
+          <t>文画学院 编著</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2655,17 +2659,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>AI 改变世界：人工智能新发展与智算经济 走向智能未来的最新探索指南</t>
+          <t>AI财务工具应用技巧：从入门到精通</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>¥39.60</t>
+          <t>¥27.60</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>方磊 黄郑</t>
+          <t>雒翠</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2682,17 +2686,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AI时代，成为强者（当当专享：印签、书签大拉页）</t>
+          <t>AI作文-小学生优秀作文大全 全国通用版3-6三四五六年级语文写作文训练辅导教材教辅 课堂优秀满分类获奖作文选范文素材大 一本解决写作难题的作文辅导书，让孩子轻松赢在作文起跑线赏，爱上写作。名师权威指导！</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>¥37.10</t>
+          <t>¥7.50</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>李尚龙 著，磨铁文化 出品</t>
+          <t>桂帜明 著</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2709,19 +2713,15 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>AI电影大制作：人人都可以成为导演 硅基物语 电影大片制作全流程指南：一本书讲透使用AI辅助电影创作核心技巧，大幅提升脚本、音乐、配音、图片、镜头和视频剪辑等工作内容效率（哪吒2大量采用了AI技术）</t>
+          <t>AI短视频创作119招：智能脚本+素材生成+文生视频+图生视频+剪辑优化 AI辅助119招，精通AI短视频生成与应用；AI剪辑，更懂您！</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>¥60.00</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>罗金海 著</t>
-        </is>
-      </c>
+          <t>¥35.90</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
           <t>page2_book23.jpg</t>
@@ -2736,17 +2736,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>AI做课：人人可做的副业 从零开始，用AI工具高效无忧做课，开启你的第二财富曲线，涵盖风尘散人、曾焱冰等成功个人做课者经验分享</t>
+          <t>AI芯片开发核心技术详解 从多年实践经验出发，系统阐述如何设计产品架构、优化软件和算法 帮助读者理解芯片相关多个模块开发的工作原理，以及应用开发的技术分析与实践</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>¥42.80</t>
+          <t>¥54.50</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>范舟 张若男 编著</t>
+          <t>吴建明、吴一昊</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2763,17 +2763,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>AI的100个关键：deepseek的底层逻辑 李尚龙著 深入浅出解读AI，从原理到应用，从挑战到机遇，带你全方位领略人工智能的精彩世界！</t>
+          <t>AI文案营销：打动人心的自媒体成交心法 爆款AI文案变现指南，从零到百万流量的100个营销案例；AI文案赚钱手册</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>¥34.90</t>
+          <t>¥33.50</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>李尚龙</t>
+          <t>王京 著</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2790,17 +2790,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>AI辅助公文写作实战：从入门到精通 从底层逻辑讲透AI辅助公文写作方法,从人机协同定位AI时代笔杆子的价值</t>
+          <t>AI绘画全面精通：软件平台+脚本文案+设计制作+案例实战 AI绘画核心技巧，一本书完全精通！60多个案例，100多分钟视频，160个干货。超值赠送：关键词、10个DeepSeek热门技巧总结、即梦与文心一格AI绘图教程</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>¥59.80</t>
+          <t>¥49.50</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>梅俊</t>
+          <t>郭珍珍</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2817,15 +2817,19 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>AI公文写作 公文写作大全 DeepSeek全场景应用 AI职场应用66问 DeepSeek 多模态AI场景应用</t>
+          <t>AI时代的点三三 讲解**全的点三三内容</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>¥37.80</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr"/>
+          <t>¥23.00</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>李劼</t>
+        </is>
+      </c>
       <c r="D28" t="inlineStr">
         <is>
           <t>page2_book27.jpg</t>
@@ -2840,17 +2844,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>AI产品经理手册 打造DeepSeek级AI产品！以AI驱动产品革新，快速学习AI技术认知和产品管理方法！</t>
+          <t>AI助力阅读：父母是孩子的英语启蒙导师</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>¥29.90</t>
+          <t>¥31.10</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>[美] 艾琳·布拉西斯（Irene Bratsis）着 张玉君 刘璐 译</t>
+          <t>敖新星</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2867,17 +2871,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>AI时代，成为强者</t>
+          <t>AI大模型 国内AI大模型的奠基之作 拥抱AI时代的到来 未来，是一场算力的竞赛</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>¥37.10</t>
+          <t>¥29.30</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>李尚龙 著，磨铁文化 出品</t>
+          <t>颜少林</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2894,17 +2898,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>AI赋能 AI恐慌难破局？领英创始人霍夫曼10大原则+全球大咖背书，教你从“焦虑”到“驾驭”！</t>
+          <t>AI公文写作高手速成：格式要点+写作技巧+模板案例 快速掌握使用主流AI工具写出高质量公文，附赠教学课件、教学视频、电子教案等资源。</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>¥66.00</t>
+          <t>¥28.70</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>[美] 里德·霍夫曼 [美]格雷格·贝亚托（Greg Beato） 著，陆坚 译，湛庐文化 出</t>
+          <t>孙建东</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2921,17 +2925,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>AI Agent开发与应用：基于大模型的智能体构建</t>
+          <t>AI风暴 : 人工智能的商业运用 《珍藏版》《畅销书》人工智能是企业发展的驱动力，掌握了人工智能的奥妙，也就洞悉了企业制胜的关键。</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>¥49.50</t>
+          <t>¥33.30</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>凌峰</t>
+          <t>孟宪坤 著 华夏智库 出品</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2948,17 +2952,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>如何向AI提问 精准提问，让DeepSeek的回答更优质 不会提问，再强大的AI工具也帮不了你。万能提问公式+超全场景对比案例，一本技术使用指南兼思维训练手册，教你学会用高效提问解锁AI“超能力”！</t>
+          <t>剪映即梦AI绘画与视频生成从入门到实践 8大Al创作核心功能+8大AI创作实战案例+4大完全配套资源+掌握DeepSeek精髓电子手册（含教学视频）</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>¥23.20</t>
+          <t>¥44.50</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>晴山 易兴 著 时代华语 出品</t>
+          <t>古月</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2975,17 +2979,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>AI动漫一本通：三分钟速通影视+动漫+设计创作</t>
+          <t>AI梦时代——月海空城</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>¥27.60</t>
+          <t>¥14.00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>李源</t>
+          <t>汪鑫</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -3002,42 +3006,42 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>AI驱动下的量化策略构建（微课视频版） 配套教学课件，100个示例源代码，213分钟视频讲解 资深量化工程师手把手教你利用AI搭建量化策略 系统讲解AI应用于投研搭建、数据挖掘、量化策略和实盘</t>
+          <t>AI时代：围棋名局名手之我见</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>¥54.50</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>江建武、季枫、梁举</t>
-        </is>
-      </c>
+          <t>¥24.00</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>page2_book34.jpg</t>
+          <t>无图片或占位图</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>output\images\page2_book34.jpg</t>
+          <t>无图片</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>AI新科技漫画人工智能deepseek前沿科技孩子爱看的趣味百科</t>
+          <t>AI数据决策：数据化决策+当我点击时，算法在想什么？（套装2册） 英国皇家学会奖学金&amp;凯瑟琳·理查兹奖得主破除AI崇拜，揭示算法黑箱本质，重塑大众对人工智能的认知?；结合全球500强企业实证的商业量化分析决策法，打造商业增长新范式，破解技术迷思与商业困局。</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>¥8.80</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr"/>
+          <t>¥83.90</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>[美]道格拉斯·W.哈伯德,[瑞典]大卫·萨普特</t>
+        </is>
+      </c>
       <c r="D36" t="inlineStr">
         <is>
           <t>page2_book35.jpg</t>
@@ -3052,17 +3056,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>AI产品经理：方法、技术与实战 一本书掌握优秀AI产品经理的产品知识、技术知识和工程化实践方法，商汤科技AI产品经理亲自执笔</t>
+          <t>你好，AI：给孩子的高效学习法（专为6至18岁孩子编写的零基础 AI 启蒙和实操书，帮助孩子从对 AI 的好奇探索，转而</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>¥72.30</t>
+          <t>¥23.20</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>王泽楷</t>
+          <t>憨爸、胡斌</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3079,17 +3083,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>AI爆款文案：AI时代的流量密码，你的心灵成长指南 李尚龙著 AI写爆款,让写作变得更快、更赚、更简单 让AI点燃你的创作灵感，轻松打造10万+爆款 AI写作变现，用AI让你的文字价值百万 教你轻松驾驭智能AI，新手小白也能成为创作大师</t>
+          <t>AI公文写作范例大全：格式、要点与技巧 AI辅助公文写作，效率飞速提升！</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>¥34.90</t>
+          <t>¥26.60</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>李尚龙著</t>
+          <t>公文先生 编著</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3106,17 +3110,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>AI战争 深入探讨了AI在军事领域的应用与风险，剖析美军军事智能现状，预测未来战争的制胜关键与挑战以及人机融合在智能战场中的合作，伦理算法决策、反人工智能和认知战等前沿议题。</t>
+          <t>AI文案写作从入门到精通 赠DeepSeek讯飞星火等AI应用指导 文心一言 chatgpt ai文章生成器 ai帮你写 115分钟同步教学视频+167个实例案例讲解，赠188页PPT教学课件+电子教案，免费领取DeepSeek、讯飞星火等国产AI大模型应用指导（附赠教学视频），AI助力，文案从此不凡！</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>¥57.70</t>
+          <t>¥29.90</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>刘伟 谭文辉</t>
+          <t>新镜界</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3133,17 +3137,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>AI辅助课题申报+AI辅助论文写作 当当套装2册</t>
+          <t>AI短视频全面应用：一键生成＋智能剪辑＋虚拟角色＋案例实操 270多个素材效果、140多分钟视频、10个DeepSeek热门技巧总结，即梦与文心一格AI绘图教程</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>¥69.80</t>
+          <t>¥49.50</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>赵鑫 宋义平 郭泽德 郭泽德 宋义平 赵鑫</t>
+          <t>岳伟</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3160,15 +3164,19 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>少年AI和狗手机里的孩子拯救天才藏起来的男孩故事之王高原水怪超凡飞手奇迹之夏尺蠖俱乐部 8-10-12岁小学生课外阅读少</t>
+          <t>AI配音全面应用：录音剪辑+字变音频+声音变字+歌曲制作 100多个实操案例、200多分钟视频、10个DeepSeek热门技巧总结，即梦与文心一格AI教程</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>¥8.10</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr"/>
+          <t>¥39.90</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>李敏</t>
+        </is>
+      </c>
       <c r="D41" t="inlineStr">
         <is>
           <t>page2_book40.jpg</t>
@@ -3183,17 +3191,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>AI系统：原理与架构陈仲铭9787030792877科学出版社</t>
+          <t>驱动AI：提示词指令入门与场景应用（人工智能前沿实践丛书） 掌握提示词技巧，与DeepSeek、ChatGPT等大模型高效协作，开启智能生活与工作新篇章！</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>¥149.25</t>
+          <t>¥44.50</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ZOMI酱,苏统华</t>
+          <t>朱晓阳</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3210,17 +3218,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>AI Agent应用与项目实战 DeepSeek大模型实战</t>
+          <t>AI摄影绘画与PS优化从入门到精通 人工智能AI绘画教程，ChatGPT指令生成+Midjourney绘画技巧+PS修图优化，人像+风光+花卉+动物+慢门+星空+航拍+全景</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>¥55.20</t>
+          <t>¥49.50</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>唐宇迪</t>
+          <t>楚天</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3237,17 +3245,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>AI全能助手：人人都能玩转DeepSeek 从入门到成为DeepSeek高手7步通关DeepSeek 解决DeepSeek应用中的各种痛点 保姆级拆解职场办公/学术研究/创意写作/生活娱乐全场景应用 深度挖掘DeepSeek的潜力</t>
+          <t>AI新媒体运营与推广从入门到精通 掌握前沿技术，洞悉市场脉动，让AI成为您的得力助手，共创营销新高度！</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>¥39.80</t>
+          <t>¥33.50</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>廖显东</t>
+          <t>叶龙</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3264,17 +3272,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>做AI时代的高手：数字化生存极简法则 数字时代的技术、工作与生存范式，技术的本质是让人类更自由地做自己，学会借势，成为AI时代的关键少数</t>
+          <t>AI大战略 人工智能如何帮助企业实现指数级增长 为你的企业找到“商业模型图”</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>¥32.60</t>
+          <t>¥37.90</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>胡荣丰、秦添 著</t>
+          <t>[美]阿莎·萨克塞纳（Asha Saxena）著，李欣瑜 译</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3291,17 +3299,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>AI时代重新定义精益管理 企业如何实现爆发式增长 智能时代 丰田精益管理中国实践方案 精益生产 精益制造系列 全书200余图表 60多个经典案例 结合作者10多年实践经验 帮助企业降本增效 获取超额利润</t>
+          <t>AI赋能短视频：爆款内容打造秘籍 解锁AI短视频新纪元，打造爆款内容，从入门到精通，一本就够！</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>¥38.30</t>
+          <t>¥44.00</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>李科 王润五 肖明涛 张林</t>
+          <t>绘蓝书源 著</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3318,15 +3326,19 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>AI辅助写作</t>
+          <t>AI新媒体运营:营销+推广实战指南</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>¥39.80</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr"/>
+          <t>¥27.60</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>彭筱星</t>
+        </is>
+      </c>
       <c r="D47" t="inlineStr">
         <is>
           <t>page2_book46.jpg</t>
@@ -3341,17 +3353,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>AI职场应用66问 DeepSeek 多模态AI场景应用 清华大学新闻与传播学院新媒体研究中心全新研究成果，AI职场应用、Deepseek实操，66个适用小技能，职场UP</t>
+          <t>AI摄影与后期制作101例（100集视频课） 10大类型+101个AI摄影案例+101个AI绘画模版+101个摄影小技巧+换脸+后期制作，Midjourney创意无限</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>¥64.20</t>
+          <t>¥39.90</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>向安玲</t>
+          <t>罗巨浪、周冰渝</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3368,17 +3380,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>AI短视频从入门到精通100例 超值赠送：DeepSeek 10个高效技巧，即梦、可灵、海螺3款AI短视频制作教程，DS+即梦、DS+剪映AI短视频的制作方法，Sora部署、登陆与视频生成实战</t>
+          <t>AI英语写作实战手册 探讨AI在英语写作中的应用，从提升写作效率到增强创作质量，重新定义创作方式</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>¥49.00</t>
+          <t>¥30.60</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>木白 编著</t>
+          <t>兰玉</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -3395,17 +3407,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>AI音乐创作从新手到高手</t>
+          <t>AI赋能的微生物组大数据挖掘:方法与应用 一部具有微生物学与生物信息学学科交叉特色，全面介绍微生物组大数据挖掘方法与应用的学术专著。</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>¥62.20</t>
+          <t>¥44.00</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>楚飞</t>
+          <t>宁康</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -3422,17 +3434,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>轻松学AI：从新手到高手</t>
+          <t>AI作文一本全搞定-中学生作文 得分策略+提分要诀+核心要素+构思导图+名师点评 初中考七八九年级优秀获奖满分高分作文范 一本解决写作难题的作文辅导书，让孩子爱上写作赢在起跑线</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>¥9.10</t>
+          <t>¥7.50</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>桂帜明</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -3449,17 +3461,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>AI提问大师 解锁公文写作的高效密码 15类常用公文场景万能提问公式 会议提要工作报告请示批复 事业单位行文 应用场景模 首本教授用AI进行公文写作的图书，15类公文场景全覆盖，5款万能公式、24种追问指令，3秒生成常用公文。赠送同步视频课、AI平台会员权限。</t>
+          <t>AI绘画与摄影实战108招：ChatGPT+Midjourney+文心一格 一本书在手，掌握多种AI绘画与摄影作品生成技巧</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>¥24.50</t>
+          <t>¥44.90</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>骆仁童 高军</t>
+          <t>石头</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -3476,17 +3488,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>AI办公从入门到精通：文字、PPT、影音 一本书提升工作效率，AI辅助WPS、PPT、剪映完全自学一本通，基础、案例、操作保姆级教学</t>
+          <t>AI+Photoshop 2025从新手到高手（微课版） 全彩印刷 超值赠送 52个视频教学文件，时长超过120分钟</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>¥69.40</t>
+          <t>¥39.50</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>宋夏成 等 编著</t>
+          <t>王庄 高连平 宋培娟</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -3503,17 +3515,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>AI+人力资源管理：HR进阶实践（新时代·管理新思维） AI+HR最大化激发人才价值，多角度赋能HR加快转型升级。AI与HR工作多个环节融合，有效推动工作流程简化优化；智能系统实现高效自动决策，贴心关怀提升员工工作体验。</t>
+          <t>AI+:人工智能时代新商业模式 人工智能时代新商业浪潮，13个AI应用领域的商业模式深度解读</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>¥33.10</t>
+          <t>¥28.70</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>梁咏峰</t>
+          <t>赵亚洲、肖军、乐粉鹏 编著</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -3530,17 +3542,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>AI时代法律人智能手册：DeepSeek实用指南( 软精装) 赵精武、翁壮壮著</t>
+          <t>AI育儿 从想法到实践</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>¥71.50</t>
+          <t>¥33.10</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>赵精武，翁壮壮 著</t>
+          <t>刘燕旎</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -3557,19 +3569,15 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>AI育儿</t>
+          <t>围棋AI定式的基本与变化</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>¥33.10</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>刘燕旎</t>
-        </is>
-      </c>
+          <t>¥26.10</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr">
         <is>
           <t>page2_book55.jpg</t>
@@ -3584,17 +3592,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>用AI做副业赚钱 快!别人都在用AI偷偷变富了! 你还在等什么? 在流量见顶的时代，还有哪些机会留给普通人？ 大白话+手把手教学，让普通人也能用AI做副业赚钱!</t>
+          <t>AI时代：图说人工智能七十年 人工智能的风云人物，里程碑事件，思维导图，音视频讲解</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>¥26.90</t>
+          <t>¥34.00</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>李牧远 著</t>
+          <t>闻新、宋华华、梁兴 编著</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -3611,17 +3619,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>AI新科技孩子超喜欢的漫画趣味百科前沿科技人工智能套装2册deepseek漫画版机器狗元宇宙智能芯片</t>
+          <t>AI营销画布：数字化营销的落地与实战 入选美国市场营销人工智能研究院“2023年AI Z佳图书”之一。数字化营销实操书籍，菲利普·科特勒“营销4.0”理论落地篇。科特勒咨询管理合伙人王赛、《流量池》作者杨飞等8位大咖联袂推荐。</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>¥22.90</t>
+          <t>¥35.60</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>师鲁贝尔</t>
+          <t>［美］拉吉库马尔·文卡特桑，［美］吉姆·莱辛斯基 著，褚荣伟，闵彦冰 译</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -3638,17 +3646,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>AI学习助手：给青少年的DeepSeek快速入门指南 专为中小学生量身打造的全学科学习神器 专为中小学生量身打造的全学科“学习神器” 家长省心省力，孩子学的开心，成绩提升轻松。</t>
+          <t>AI智能办公：ChatGPT+Office+WPS应用从入门到精通 AI火力全开，助力职场智能新时代。</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>¥25.00</t>
+          <t>¥35.10</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>图蓝 赛启团队 著 王娜 绘</t>
+          <t>徐捷、雷鸣 编著</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -3665,17 +3673,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>AI短视频生成与剪辑实战108招：ChatGPT+剪映 赠送Deepseek、即梦、可灵、kimi、通义、文心一言、秘塔等工具的使用指导，70多个案例关键词+108招干活技巧，实操实练，秒变AI视频高手</t>
+          <t>AI创意绘画与视频制作：基于Stable Diffusion和ControlNet 带你创作更高品质的图像与动画，释放无限创意，探密更前沿的AI绘画技巧。Stable Difussion绘画、AI绘画、ControlNET、AI动画</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>¥44.90</t>
+          <t>¥59.50</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>蒋珍珠</t>
+          <t>马健健</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -3692,17 +3700,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>AI繁荣 以多场景真实案例破除AI威胁论，展现正向价值；融合人文视角，探讨技术对情感社交、伦理安全的影响；借虚构人物故事让AI经济学通俗易懂。</t>
+          <t>AI作文-小学生作文大全 老师推荐三3四4五5六6年级语文写作文训练辅导教材教辅 课堂优秀满分类获奖作文选范文素材大全 一本解决写作难题的作文辅导书，好作文由好方法，一本全搞定！让孩子轻松赢在作文起跑线上，爱上写作！</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>¥50.50</t>
+          <t>¥7.50</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>艾宁德亚·高斯 拉维·巴普纳</t>
+          <t>桂帜明</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -3765,17 +3773,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>用DeepSeek赚钱（AI变现实操） 普通人用AI赚钱，根本不需要懂技术。21个真实案例，教你用DeepSeek躺赚。不学提示词、不养账号、不写代码,立即上手，毫无门槛。涵盖自媒体、电商、技能变现、线下实体等诸多场景。</t>
+          <t>AI向善：以人为中心的人工智能 美国国家工程院院士重磅力作，探索DeepSeek时代机器与人类的共生之道!</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>¥21.20</t>
+          <t>¥40.10</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>水青衣 焱公子 著 时代华语 出品</t>
+          <t>[美]本·施耐德曼（BenShneiderman）</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -3792,17 +3800,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AI赋能小红书运营：爆款打造+推广引流+店铺运营+品牌战略+实操案例 以Deepseek等AI工具结合小红书算法等专业运营，实现从0到1运营小红书</t>
+          <t>解锁AI职场超能力：从撰写提示词到9大场景应用 用AI高效工作，打造职场核心竞争力 人人都能掌握的AI赋能法则，揭秘8大提示词要素，9大工作场景应用，30+全球热门AI工具，100+人机实景对话演示，助你让AI成为职场的超级助手，从入门到精通。</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>¥28.70</t>
+          <t>¥35.90</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>符健治</t>
+          <t>智趋编写组</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -3819,17 +3827,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AI赋能演讲：关键时刻讲出影响力（新时代·职场新技能） 8种关键演讲场景；50+表达模型；100+应用实例精华。 AI赋能演讲，全面提升你的演讲逻辑力与说服力！</t>
+          <t>AI绘画+LoRA模型训练从新手到高手 全彩印刷 附送15集教学视频，时长超过130分钟</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>¥33.10</t>
+          <t>¥49.50</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>田楠 著</t>
+          <t>刘双亚，朱翔宇</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -3846,17 +3854,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>夸克AI 高效学习法 毕业于北大、清华的资深AI应用专家和教育科技专家撰写，北大、上海交大等10余名校名师联袂推荐，提供全面AI学习方法</t>
+          <t>AI时代围棋新定式揭秘 不可不知的智能时代围棋新技术，*AI定式助你提高围棋水平</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>¥53.70</t>
+          <t>¥21.60</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>乔剑 苏小文 王琛珏</t>
+          <t>李道宏</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3873,15 +3881,19 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AI绘画AI写作人工智能系列书籍</t>
+          <t>AI作文-小学生满分作文大全 得分策略+提分要诀+核心要素+构思导图+名师点评 老师推荐优秀获奖满分类作文素材三3四4五 一本解决写作难题的作文辅导书，让孩子轻松赢在作文起跑线上，爱上写作。</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>¥32.50起</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+          <t>¥7.50</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>桂帜明</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>page3_book5.jpg</t>
@@ -3896,17 +3908,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AI动漫角色设定教程 用Midjourney做角色设计，跟着做，自己的角色立等可取！不需绘画基础，附赠教学视频方便学习，完整讲解AI角色设计的思路、流程，包含角色、场景、世界观！</t>
+          <t>AI一键PPT实用案例 AI辅助提高PPT设计能力，快速搞定演讲、汇报、总结、商务、视觉展示PPT。</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>¥62.20</t>
+          <t>¥44.60</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>芝士冻</t>
+          <t>绘蓝书源 著</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3923,17 +3935,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AI提问之道：不会提问，怎么玩AI ai书籍、ai提问、ai交互、chatgpt、kimi、ai提示词、提示工程、pro</t>
+          <t>给孩子的AI启蒙书</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>¥29.90</t>
+          <t>¥34.00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>杜光明</t>
+          <t>李丹</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3950,17 +3962,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>AI革命：人工智能如何为商业赋能 AI革命：人工智能如何为商业赋能</t>
+          <t>AI绘画+AI电商广告制作从入门到精通 赠DeepSeek即梦可灵等AI应用指导 ai人工智能实战 ChatGPT Mi 75分钟同步教学视频+123个实例讲解，赠5200例绘画及提示词，免费领取DeepSeek、即梦、可灵等AI应用指导（附赠教学视频）</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>¥43.50</t>
+          <t>¥39.90</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[美]尼尔·萨霍塔 迈克尔·阿什利</t>
+          <t>新镜界</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -3977,17 +3989,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>AI觉醒：生成式人工智能产业机遇与数字治理 鲁俊群 李璇 人工智能+赋能加快形成新质生产力，洞察以AIGC和ChatGPT为代表的大模型驱动社会、商业和生活的关键。中国工程院院士倪光南、陈清泉，知名专家学者孙茂松、吴飞、马维英、胡志坚联袂推荐！</t>
+          <t>AI改变设计——人工智能时代的设计师生存手册 洞察AI时代设计领域的发展，找准定位，实现价值！</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>¥39.50</t>
+          <t>¥34.50</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>鲁俊群 李璇</t>
+          <t>薛志荣</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -4004,17 +4016,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>AI帮你赢人人都能用的AI方法论 实用的AI学习法，与人工智能交互第一性原理，从提示词到超级个体，周鸿祎作序推荐</t>
+          <t>AI文生视频：Sora引领内容变革浪潮 深度剖析文生视频底层逻辑，全面盘点AI视频平台及工具。Sora颠覆传统视频创作模式，AI产业链迎来重大机遇期。文生视频模型落地场景广泛，智能化水平推动多领域变革</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>¥54.40</t>
+          <t>¥39.50</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>谭少卿</t>
+          <t>徐鹏 常亮</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -4031,17 +4043,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AI助力教学：让中小学教师工作更高效</t>
+          <t>AI绘画全场景案例应用与实践 彩色印刷,58个案例,用SD3,可图,混元和Flux等新模型实现案例效果,赠教学视频,训练集,提示词库,PPT等,QQ群,B站,E-mail,公众号售后</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>¥49.50</t>
+          <t>¥43.10</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>黎渝幸 著</t>
+          <t>王双、王佑琳、朱美霞</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -4058,17 +4070,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AI提示工程必知必会 让AI成为你的高效助理，用好DeepSeek提示词，走上开挂人生，适合各层次读者</t>
+          <t>AI降临：ChatGPT实战与商业变现 ChatGPT助力掘金，一个人的超级团队时代来临！</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>¥44.50</t>
+          <t>¥49.00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>王国平</t>
+          <t>张永刚、杜一凡、欧阳军 编著</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -4085,19 +4097,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AI辅助编程Python实战基于GitHub Copilot和ChatGPT 深度剖析AI辅助编程，以Copilot为切入点，结合Python实战案例，助力读者快速掌握函数设计、代码测试与自动化开发等核心技能。</t>
+          <t>全2册 AI漫画人工智能新时代+漫画前沿新科技（平装）科技改变生活孩子超喜欢的漫画趣味百科让孩子从小对科技产生兴趣 提高</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>¥44.90</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>[美] 利奥·波特（Leo Porter）[加] 丹尼尔·津加罗（Danie</t>
-        </is>
-      </c>
+          <t>¥13.50</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
           <t>page3_book13.jpg</t>
@@ -4112,17 +4120,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>AI落地：让人工智能为你所用 王海屹 企业构建人工智能运营能力、个人提升科学素养和技能的实用指南！科普+强启发性，分析如何在各行各业赋能落地应用。无技术基础、看不懂公式的人也适用！共读的人越来越多，快来加入驾驭AI的队伍！霍夫曼推荐</t>
+          <t>AI数字人从制作到商用：电商带货+视频教学+广告营销+生活服务 AI数字人制作与直播商用从入门到精通</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>¥39.50</t>
+          <t>¥44.00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>王海屹</t>
+          <t>伏龙 编著</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -4139,44 +4147,40 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>AI营销画布 数字化营销的落地与实战 中国科学技术出版社 新华书店正版，关注店铺成为会员可享店铺专属优惠，团购客户请咨询在线客服！</t>
+          <t>围棋AI评吴清源</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>¥27.10</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>(美)拉吉库马尔·文卡特桑,(美)吉姆·莱辛斯基</t>
-        </is>
-      </c>
+          <t>¥60.00</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>page3_book15.jpg</t>
+          <t>无图片或占位图</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>output\images\page3_book15.jpg</t>
+          <t>无图片</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>AI领导课：企业数智化转型的9项关键行动 出色AI领导力的实战密码，9大关键行动指南，从"AI小白"到战略舵手！聚焦企业数智化转型，让AI成为组织的增长引擎，实现协同进化共赢</t>
+          <t>AI智能陪练：车尔尼599钢琴初级教程（超大开本，超大音符，平铺乐谱更便于弹奏，乐谱与教学视频相对照，直观体验弹琴的基本</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>¥33.50</t>
+          <t>¥17.10</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>[比]大卫 · 德克莱默（David De Cremer）</t>
+          <t>谈天佳</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -4193,17 +4197,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>AI时代Python量化交易实战：ChatGPT让量化交易插上翅膀 关东升 韩文锋 金融量化交易新模式：一本专注于帮助交易师在AI时代实现晋级、提高效率的图书。书中介绍了如何使用 ChatGPT 来完成量化交易的各个环节，并通过实战案例展示了ChatGPT在实际量化交易中的应用方法。</t>
+          <t>用DeepSeek赚钱（AI变现实操） 普通人用AI赚钱，根本不需要懂技术。21个真实案例，教你用DeepSeek躺赚。不学提示词、不养账号、不写代码,立即上手，毫无门槛。涵盖自媒体、电商、技能变现、线下实体等诸多场景。</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>¥43.50</t>
+          <t>¥21.20</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>关东升,韩文锋 编著</t>
+          <t>水青衣 焱公子 著 时代华语 出品</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -4220,17 +4224,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>AI智能写作助手：创作技巧、内容优化与科研应用 AI辅助论文写作，AI提示词高效使用范例大全；ChatGPT学术创作技巧</t>
+          <t>AI场景革命 生成式人工智能Sora、Kimi强势“出圈” 空间计算时代如何打造爆款场景模型</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>¥30.60</t>
+          <t>¥39.50</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>王常圣、李强、汪正斌 著</t>
+          <t>焦娟、罗中天、王利慧、石昊楠、周昭</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -4247,17 +4251,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>剪映AI：短、中、长视频剪辑全攻略（手机版+电脑版+网页版） AI赋能剪映，3秒智能成片，7步专业级制作；一个软件，三个版本，三种视频，全面精通。</t>
+          <t>剪映AI视频剪辑：AI脚本+AI绘画+图文生成+数字人制作 AI剪映从入门到精通；AI短视频教程；剪映剪辑</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>¥44.90</t>
+          <t>¥44.00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>沈沛</t>
+          <t>龙飞 编著</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -4274,17 +4278,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>AI智能办公实战108招：ChatGPT+Word+PowerPoint+WPS 赠送Deepseek、即梦、可灵、kimi、通义、文心一言、秘塔等工具的使用指导，一本书在手，AI智能办公信手拈来</t>
+          <t>AI设计与创意实战：品牌、空间、叙事与艺术的未来融合 AI设计AI绘画AI视频实战、品牌、空间、广告视觉创意Midjourney AI技术应用案例解析</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>¥44.90</t>
+          <t>¥47.50</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>曾公子</t>
+          <t>郭爽 编著</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -4301,17 +4305,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>AI赋能的数字化营销管理</t>
+          <t>剪映+AI短视频剪辑从入门到精通（手机版+电脑版+网页版）剪映AI、短视频剪辑、剪映书、剪映教程、视频处理软件、抖音快手</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>¥41.40</t>
+          <t>¥34.90</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>刘毅</t>
+          <t>新镜界</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -4328,17 +4332,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AI赋能：大模型概念、技术及企业级项目应用 田野 张建伟 联想方案服务业务集团大模型与智能体项目实践经验总结，详解大模型三种建设路径及六类应用模式，大模型选型建设标准及项目实施方法</t>
+          <t>AI高效办公：用Python三分钟搞定全天工作</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>¥72.30</t>
+          <t>¥27.60</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>田野 张建伟</t>
+          <t>李长玖</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -4355,17 +4359,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>零基础开发AI Agent——手把手教你用扣子做智能体 DeepSeek大模型适用</t>
+          <t>超级AI与未来教育 30个痛点问题，解读未来教育大趋势，学会提问，在AI时代让教育更美好，顾明远、朱嘉明、段永朝、李睦、李政涛、李志民等十余位专家学者联袂推荐</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>¥55.00</t>
+          <t>¥35.60</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>叶涛</t>
+          <t>李骏翼</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -4382,17 +4386,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>AI群星闪耀时 清华大学计算机副教授刘知远作品，28段传奇人生，18张清华美院的手绘图，还原人工智能历史发展篇章，人类群星闪耀时AI版</t>
+          <t>AI多媒体：AI脚本+AI绘图+AI视频+AI音乐商用实战100例</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>¥34.90</t>
+          <t>¥27.60</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>刘知远 曾哲妮</t>
+          <t>金李娜</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -4409,17 +4413,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>AI写作：爆款文案从入门到精通 一本书精通ChatGPT、文心一言两大AI文案创作工具！快速掌握AI文案写作180招，获取爆款文案创作灵感！超值赠送教学视频、DeepSeek应用技巧及教学课件</t>
+          <t>AI辅助海报设计101例（关键词+设计思路+心得体会） 101个AI海报设计案例，助力读者开拓思维，激发灵感，提高效率！</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>¥28.70</t>
+          <t>¥49.90</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>叶龙</t>
+          <t>罗巨浪、陈静茹</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -4436,17 +4440,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>AI沟通力：沟通就是这么简单（漫画图解版） 说话也是个技术活，像高手一样接话和回话，漫画图解×AI工具，化解沟通难题，建立真诚愉悦的社交关系，提升个人竞争力，附赠AI训练手册。</t>
+          <t>AI英语家教:三个月精通听说读写</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>¥33.90</t>
+          <t>¥27.30</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>峥嵘</t>
+          <t>张佳佳</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -4463,17 +4467,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>AI短视频创作与剪辑从入门到实践(微视频版) 随书提供书中案例操作视频、素材文件等配套资源，获取地址见书内容简介网址，或前言和封底二维码。教材服务QQ：1815317009。</t>
+          <t>AI源码解读：数字图像处理案例（Python版）（人工智能科学与技术丛书） 融汇科研与教学经验，案例可二次开发利用！阿里巴巴|字节跳动|讯飞智元|腾讯|百度|微软 专家联袂推荐！配套程序代码、工程文件、附赠案例！</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>¥44.50</t>
+          <t>¥59.50</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>李莹、宋岩峰、王嘉熠</t>
+          <t>李永华</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -4490,17 +4494,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>AI效率手册：从ChatGPT开启高效能 构建一个完整的AI学习体系，知乎头部大V出品，掌握使用AI的方法，融合AI场景，助力效率力、学习力全面提升</t>
+          <t>AI商业化 人工智能、AI、企业经营、数字化时代</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>¥39.90</t>
+          <t>¥20.90</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>常青</t>
+          <t>（日）石川聪彦</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -4517,17 +4521,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>AI销冠：一个人顶一个团队的销售术 唐兴通 AI时代销售实现持续爆单的秘籍，IBM、SAP、西门子、思科、梅特勒-托利多的高管鼎力推荐</t>
+          <t>AI商业应用落地 AI商业应用落地，开启商业新纪元</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>¥60.50</t>
+          <t>¥33.50</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>唐兴通</t>
+          <t>肖忠海、陈耿宣 著</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -4544,17 +4548,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>零基础学AI编程（项目实战版）――DeepSeek + Cursor 不需要编程基础，就能学习。 “DeepSeek + Cursor”双工具——利用DeepSeek落地创意，利用Cursor快速落地代码 5种应用类型全覆盖：网页、小程序、在线游戏、桌面应用、超市商城</t>
+          <t>AI源码解读：循环神经网络（RNN）深度学习案例（Python版） 阿里巴巴|字节跳动|腾讯|百度|微软专家联袂推荐！利用Python编程实现深度学习经典案例！融汇丰富科研与教学经验！</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>¥49.00</t>
+          <t>¥44.50</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>罗健</t>
+          <t>李永华 曲宗峰 李红伟</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -4571,17 +4575,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>AI绘画大师Midjourney：写给小白的100种应用 手把手教你Midjourney实战的基础与进阶，迸发艺术灵感，创造无限可能！免费提供1.2万多个提示词，一秒出图、0理论全实践，一本艺术与科技结合的百科全书。</t>
+          <t>AI图景：Sora时代的人工智能应用 把握时代脉搏，预见DeepSeek未来，揭示人工智能实践新思路。</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>¥101.50</t>
+          <t>¥30.60</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>文之易</t>
+          <t>[美]阿莉莎·辛普森·罗赫韦格（AlyssaSimpsonRochwerger）,[美]逄伟（WilsonPang） 著</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -4598,17 +4602,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>探源--AI狂飙时代的管理常识与实践创新 追问商业与社会的本质逻辑，解读AI时代的破局思维与生存法则</t>
+          <t>AI应用高效实操大全：生活咨询+办公文案+绘画设计+音视频创作 123种实战案例，16种提问技巧，AI应用高效实操大全一本就够！</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>¥49.10</t>
+          <t>¥31.10</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>吴晨 著</t>
+          <t>王晓蕾、姜旬恂、王悠 著</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -4625,17 +4629,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>AI+3ds Max 2025从新手到高手（微课版） 全彩印刷 72个视频，时长超过7小时</t>
+          <t>AI文案高手速成118例：提问生成+修改润色+热门模板+应用案例</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>¥49.50</t>
+          <t>¥29.50</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>来阳</t>
+          <t>AIGC文画学院 编著</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -4652,17 +4656,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>海螺AI短视频创作全攻略：一键生成你的视频大片 海螺AI一键生成你的视频大片，爆款短视频创作全掌握！</t>
+          <t>AI助力Python编程做与学 人工智能让Python飞起来，简短代码高效解决大问题</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>¥61.60</t>
+          <t>¥49.50</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>王占坤 著</t>
+          <t>李金洪 主编 韩博、王细薇 副主编</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -4679,19 +4683,15 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>国产AI大模型DeepSeek实战操作指南入门搜索答疑写作黄豆奶爸DeepSeek实操指导手册普及知识读物零基础小白也能</t>
+          <t>AI时代的老年生活 身处AI时代，老后的我们会遇到哪些问题？当你老了，AI可以帮你！</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>¥35.80</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>黄豆奶爸</t>
-        </is>
-      </c>
+          <t>¥26.10</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
           <t>page3_book35.jpg</t>
@@ -4706,17 +4706,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>AI短视频创作一本通： 剪映+即梦+即创+可灵+腾讯智影+文心一言+AI数字人 6大AI工具，·49个实战案例，470多张图片，AI短视频制作全掌握！</t>
+          <t>AI时代，学什么，怎么学 清华大学理学博士、人大附中和渊老师解读AI时代学习法，教你掌握未来世界核心竞争力，该如何正确、有效地使用人工智能工具，无需焦虑，这本书让你不掉队。</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>¥39.00</t>
+          <t>¥39.90</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>郝倩 著</t>
+          <t>和渊</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -4733,17 +4733,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>AI新个体：用DeepSeek重塑一人公司 用AI开启你的自由副业，在家也能创办一人公司，一人公司2.0模式正式开启，让AI成为你的第二大脑，重构变现模式，升级认知系统，做AI时代的超级个体</t>
+          <t>AI绘画师：文案、图片与视频制作从入门到精通 AI；ChatGPT；Midjourney;AIGC;剪映；文心；</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>¥29.90</t>
+          <t>¥44.00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>鱼堂主</t>
+          <t>AIGC文画学院 编著</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -4760,17 +4760,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>AI短视频创作攻略 剪映、即梦AI、Deepseek等视频创作技巧全应用，赠140多分钟教学视频，素材、指令随书附赠</t>
+          <t>AI创意商业广告设计：Adobe Firefly + Photoshop AI创意商业广告设计：Adobe Firefly + Photoshop</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>¥54.60</t>
+          <t>¥64.50</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>AI技能提升工作组 编著</t>
+          <t>王红卫</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -4787,17 +4787,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>AI短视频高手速成：一键生成与剪辑 隐军 让所有人成为AI短视频高手，一键成片！赠送160分钟视频教程、全套视频素材，Deepseek、海螺、Sora使用教程</t>
+          <t>AI活动策划与执行大全 从需求分析到文案策划、从活动执行到效果评估,全程AI精准赋能,助您抢占市场先机。</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>¥34.50</t>
+          <t>¥29.80</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>隐军</t>
+          <t>叶龙</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -4814,17 +4814,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>AI教育行业应用从入门到精通 多种配套资源，30多个AI教育工具，搭配80个实战案例解析。</t>
+          <t>AI提示词工程师：精通ChatGPT 提问与行业热门应用208例 一本书精通ChatGPT提问与提示词热门应用，赠送教学视频+关键词+素材效果！</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>¥28.70</t>
+          <t>¥34.00</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>谭先</t>
+          <t>文画学院 编著</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -4841,17 +4841,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>AI剪辑师手册：剪映短视频制作从入门到精通 一本书精通剪映AI热门短视频制作 超值赠送：DeepSeek 10个前沿使用技巧，Kimi等7款国产免费的AI工具文案写作方法，即梦、文心一格绘画的方法，即梦、可灵、海螺3款AI短视频制作教程</t>
+          <t>AI+ART 中国人工智能学会系列研究报告 人工智能给艺术带来更多创新和可能，本书将带你领略AI+ART的领域的魅力</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>¥49.00</t>
+          <t>¥44.60</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>木白 编著</t>
+          <t>邱志杰，等</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -4868,17 +4868,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>少年AI和狗 2024高考作文热点素材 大白鲸科幻世界【十三五国家重点出版物出版规划项目】中小学生课外阅读儿童太空科幻书 新华书店正版，关注店铺成为会员可享店铺专属优惠，团购客户请咨询在线客服！</t>
+          <t>昇腾AI处理器架构与编程-深入理解CANN技术原理及应用 华为智能计算机技术丛书 华为官方授权 华为公司出品！华为轮值董事长徐直军、中国工程院院士高文、中国科学院院士毛军发作序！揭开达芬奇架构AI处理器的神秘面纱、掌握强大算力的使用方法！</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>¥12.90</t>
+          <t>¥34.50</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>杨华</t>
+          <t>梁晓峣</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -4895,17 +4895,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>AI赋能HR：AI 10倍提升HR工作效率的方法与实践 田政 谷燕燕 唐琨 资深专家撰写，系统梳理AI赋能HR的43个场景，通过科学方法、高效提示词、详细步骤、丰富案例手把手教HR用AI</t>
+          <t>可灵AI视频与AI绘画技巧大全 可灵AI视频生成技巧；即梦AI海螺AI通用视频生成教程；AI视频制作剪辑一本通</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>¥72.30</t>
+          <t>¥35.90</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>田政 谷燕燕 唐琨</t>
+          <t>龙飞 编著</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -4922,17 +4922,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>AI公文写作：理念、方法与实务 你的工作其实能一键生成。把耗时间的事、麻烦的事、重复的事都丢给AI，让公文写作效率倍增</t>
+          <t>AI绘画师：电商产品文案+广告＋模特＋视频制作全攻略 ChatGPT；Midjourney;</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>¥47.50</t>
+          <t>¥39.00</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>胡森林</t>
+          <t>AIGC文画学院 编著</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -4949,17 +4949,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>AI化学与生物 口袋里的人工智能 人工智能知识启蒙科普读物 AI技术应用化学生物应用化学合成蛋白质结构基因调控新材料预测 从大众科普的角度，对人工智能在化学、生物领域的应用进行了阐述</t>
+          <t>AI绘画101例——小白上手宝典全彩视频 AIGC绘画师从入门到精通 AIGC设计创意实战 零基础玩转AI绘画 midj 基于Midjourney、Stable Diffusion等软件的AI绘画零基础入门书，通过案例，探索AI绘画的魅力，享受创作的乐趣，发掘创作的潜能。</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>¥16.60</t>
+          <t>¥59.00</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>陈俊龙 马晶</t>
+          <t>殷娅玲 李虹霖</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -4976,17 +4976,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>剪映+AI：爆款短视频文案 素材 剪辑 特效一本通 AI制作短视频方法入门，DeepSeek、即梦、豆包等AI工具助力文案生成、素材生成、后期剪辑、添加特效，附赠案例素材和教学视频。</t>
+          <t>AI源码解读：机器学习案例（Python版） 融汇科研与教学经验，案例可二次开发利用！阿里巴巴、字节跳动、讯飞智元、腾讯、百度、微软专家联袂推荐！配套程序代码、工程文件、问题解疑、实战案例！</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>¥38.90</t>
+          <t>¥54.50</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>李延周</t>
+          <t>李永华</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -5003,17 +5003,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>超能助手AI机器人/大冒险家辛巴狗 勇闯世界，探索未知！原创国漫辛巴狗，作者欧阳宏利倾力打造！穿梭于虚拟与现实的奇幻冒险，融入科技，历史，现代科技的寻宝之旅，传递友情、勇气、责任！激发孩子创造力、想象力，点燃每个孩子的英雄梦！</t>
+          <t>AI绘画从指令到制作一本通 抓住AI风口，零基础也可以创作美术作品，不用请设计师，就可以轻松搞定店铺运营的美工工作</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>¥17.80</t>
+          <t>¥39.60</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>欧阳宏利</t>
+          <t>李凤 编著</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -5030,17 +5030,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>AI写作:用AI倍速提升写作效率</t>
+          <t>少年学AI：我的第一本人工智能实战手册 探索AI世界，开启未来之门！写给青少年的人工智能启蒙与实践书</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>¥46.20</t>
+          <t>¥26.60</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>邓世超</t>
+          <t>雷波 编著</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -5057,17 +5057,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>AI办公助手 ChatGPT+Office智能办公从入门到实践（80集视频课） 人工智能时代，AI+ChatGPT助力Word、Excel、PPT智能高效办公，提高工作效率，提升职场竞争力</t>
+          <t>剪映AI短视频+虚拟数字人制作实操大全</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>¥39.90</t>
+          <t>¥35.60</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>宫祺</t>
+          <t>构图君</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -5084,17 +5084,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>AI动漫游戏绘画设计 精选200多个游戏动漫方向的项目案例，全方位展示Midjourney 在游戏动漫行业中的应用。</t>
+          <t>我的AI弟弟【3-8岁】人工智能启蒙绘本 3个趣味故事普及人工智能的概念 激发孩子好奇心 北京大学智能学院教授审读推荐 阅读精彩童话故事，探索奇妙科普知识，立足未来的人工智能科普绘本。每册3个趣味故事，有用的人工智能科普知识，激发孩子想象力！给孩子讲述人工智能概念的前沿科学启蒙读物，北大教授审读推荐。</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>¥53.00</t>
+          <t>¥19.10</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>王星儒</t>
+          <t>闵小玲</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -5111,17 +5111,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>AI陪你学信奥：CCF CSP认证通关实训 资深信奥教练倾力打造,紧扣CCF CSP-J/S认证标准,引入AI辅助学习模式,赠送视频课程、考纲、真题等大量资源。</t>
+          <t>MCP协议与AI Agent开发：标准、应用与实现 详解MCP技术精髓，融合DeepSeek平台能力，赋能智能系统高效开发与复杂任务落地。</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>¥54.40</t>
+          <t>¥49.50</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>刘增杰 王少华 柳华盛</t>
+          <t>凌峰、王伊凝</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -5138,17 +5138,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>AI for Science：人工智能驱动科学创新 展现人工智能驱动科学创新AI for Science与材料科学、生命科学、电子科学、能源科学、环境科学交叉融合的蓝图</t>
+          <t>少年学AI，看这本就够了 零基础掌握DeepSeek 人工智能入门与实战书籍 青少年编程思维训练 机器学习实战 未来科技</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>¥49.00</t>
+          <t>¥29.80</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>杜雨</t>
+          <t>武育泰</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -5165,17 +5165,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>AI大模型开发之路：从入门到实践 内容全面，由浅入深，实战案例丰富，一本全面探索人工智能大模型开发领域的实用指南</t>
+          <t>AI时代学什么怎么学 解读AI时代学习法 掌握未来核心竞争力 不被淘汰 和渊著 高盈绘 如何领先一步转变思路 家庭教育育 新华书店正版，关注店铺成为会员可享店铺专属优惠，团购客户请咨询在线客服！</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>¥44.90</t>
+          <t>¥35.60</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>谢雪葵</t>
+          <t>和渊</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -5192,17 +5192,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>这就是AI智能体——AI Agent入门 由浅入深地讲解AI智能体 兼顾零基础人群和有技术基础的人群 配有思维导图和图解</t>
+          <t>解密AI绘画与修图：Stable Diffusion+Photoshop 从基础操作到进阶玩法，从交互应用到行业案例，将为你提供全面的学习指南。</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>¥46.60</t>
+          <t>¥44.50</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>张梓铭（@北茗）</t>
+          <t>王岩 王希竹</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -5219,17 +5219,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>AI数字孪生建模与计算 基于AI和物理模型集成，从动态视觉全面、深入介绍建模，填补了数字孪生领域空白，并为模型可解释性提供了新范式。参考文献请扫封底二维码下载。</t>
+          <t>AI通识课12讲：走进人工智能 12堂硬核通识课，拆解AI感官、思维与创造力，重构教育、就业与人性认知！</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>¥34.00</t>
+          <t>¥52.00</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>[美] 兰詹·甘古里, 桑迪蓬·阿迪卡里, 苏维克·查克拉博蒂, 姆里蒂卡·甘古利</t>
+          <t>包坤</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -5246,17 +5246,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>秒懂AI提问：让人工智能成为你的效率神器 精心提炼20种GPT提问方法及指令，从入门到进阶再到精通，100个案例带你玩转GPT，掌握高效AI提问方法，充分发挥GPT威力，好问题才有好答案</t>
+          <t>AI作文-小学生小考满分作文大全 得分策略+提分要诀+核心要素+构思导图+名师点评 小升初优秀作文素材大全三3四4五5六 名师权威指导 教师推荐用书好方法+学范例=高分作文</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>¥29.90</t>
+          <t>¥7.50</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>秋叶 刘进新 姜梅 定秋枫</t>
+          <t>桂帜明 著</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -5273,17 +5273,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>剪映即梦AI绘画与视频生成从入门到实践 8大Al创作核心功能+8大AI创作实战案例+4大完全配套资源+掌握DeepSeek精髓电子手册（含教学视频）</t>
+          <t>AI营销：人工智能助力销售破局</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>¥44.50</t>
+          <t>¥27.60</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>古月</t>
+          <t>唐跃英</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -5300,17 +5300,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>你好，AI：给孩子的高效学习法（专为6至18岁孩子编写的零基础 AI 启蒙和实操书，帮助孩子从对 AI 的好奇探索，转而</t>
+          <t>漫画版我的第一本AI入门书零基础学AI全套2册 培养孩子AI知识巩固AI基础认知中小学人工智能课外读书书籍零基础秒懂</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>¥23.20</t>
+          <t>¥20.40</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>憨爸、胡斌</t>
+          <t>陈静芬</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -5327,17 +5327,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>AI大模型重塑现代银行 银行的变革与实践，系统解读银行业迈入 系统、全面解析AI人工智能在银行业应用与实践的著作。系统解读银行业迈入AI新时代，把握数智革命下的行业新引擎。</t>
+          <t>AI探视人类情感原理与实践——人工智能驱动的音乐信息检索 声学信号处理、语音自动识别、自然语言理解、资源检索与发现、自然语言生成、语音合成等，其中内容检索是满足用户终需求的关键技术。可以把音乐看成一种特殊的、带有情感的、更高维度的“语言”，对此进行研究可以</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>¥43.50</t>
+          <t>¥44.50</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>毕超，刘鑫</t>
+          <t>秦静</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -5354,17 +5354,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>AI加速器架构设计与实现 地平线BPU首席架构师/英伟达前高级架构师15年经验总结，图解NPU算法、架构与实现，从零设计产品级加速器</t>
+          <t>AI时代能力修炼(走进日本) AI时代你必须修炼的生存能力！修炼逆境观，学通共情秘籍，掌握夜间成长法，转AI失业危机为能力修炼良机，穿越AI革命风暴，超越经验型智慧，拥抱AI时代的大变革！</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>¥72.30</t>
+          <t>¥19.00</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>甄建勇 王路业 著</t>
+          <t>[日]田坂广志 著; 魏海波 陈海燕 译</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">

</xml_diff>